<commit_message>
Atualização, removido Thread, adicionado scroll genérico
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/hub/bdd/testdata/TestData.xlsx
+++ b/src/test/java/br/com/rsinet/hub/bdd/testdata/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-bdd\src\test\java\br\com\rsinet\hub\bdd\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilker.nogueira\eclipse-workspace-automacao\avaliacao-automacao-bdd-appium-hub\src\test\java\br\com\rsinet\hub\bdd\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D38CE80-06CB-453F-A4CE-165D3E5ED31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7075AA0B-4ACD-4CB8-868A-E303AAB09362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{8A0BD1D9-DBE4-467F-9B03-07923CE60D62}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>Wbn221190</t>
   </si>
@@ -223,9 +223,6 @@
     <t>headphones</t>
   </si>
   <si>
-    <t>laptops</t>
-  </si>
-  <si>
     <t>Validação</t>
   </si>
   <si>
@@ -244,12 +241,6 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>HP ENVY x360 - 15t Laptop</t>
-  </si>
-  <si>
-    <t>HP ENVY X360 - 15T LAPTOP</t>
-  </si>
-  <si>
     <t>C(2,0) P(2,1) V(2,2)</t>
   </si>
   <si>
@@ -289,7 +280,16 @@
     <t>C(13,0) V(13,1)</t>
   </si>
   <si>
-    <t>Wilkerbn502</t>
+    <t>Geral</t>
+  </si>
+  <si>
+    <t>No results for</t>
+  </si>
+  <si>
+    <t>C(14,0) v(14,1)</t>
+  </si>
+  <si>
+    <t>Wilkerbn503</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F037193-F877-43F4-BA53-AC2F28E12A40}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,10 +1140,10 @@
         <v>57</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,13 +1151,13 @@
         <v>61</v>
       </c>
       <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,27 +1165,27 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>70</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,26 +1193,26 @@
         <v>58</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -1222,10 +1222,10 @@
         <v>56</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1236,28 +1236,39 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>